<commit_message>
feat Upd excel backup
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/ConsultaVehicularSoat.xlsx
+++ b/src/test/resources/dataDriven/ConsultaVehicularSoat.xlsx
@@ -3,23 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/candyespinzabaez/Documents/Android/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ProyCanalApp/Android/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056EC55B-27E9-4E41-835B-81991AA56572}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2381547C-7227-7547-91B6-46070A0508D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3420" windowWidth="26000" windowHeight="16980" activeTab="2" xr2:uid="{897FEA26-AEC5-9349-951A-1C74BA5F166B}"/>
+    <workbookView xWindow="7200" yWindow="5020" windowWidth="26000" windowHeight="10460" activeTab="3" xr2:uid="{897FEA26-AEC5-9349-951A-1C74BA5F166B}"/>
   </bookViews>
   <sheets>
     <sheet name="Indice" sheetId="16" r:id="rId1"/>
     <sheet name="DescargaPolizaVehicularDigital" sheetId="19" r:id="rId2"/>
-    <sheet name="TiempoInactividadConsultaVehicu" sheetId="20" r:id="rId3"/>
+    <sheet name="ConsultaNumeroDePolizaVehiSoat" sheetId="21" r:id="rId3"/>
+    <sheet name="ConsultarDeudasSaldosdePoliza" sheetId="22" r:id="rId4"/>
+    <sheet name="TiempoInactividadConsultaVehicu" sheetId="20" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>usar</t>
   </si>
@@ -80,14 +82,37 @@
     <t>Esperar 15 min de inactividad en el modulo de Consulta Vehicular SOAT</t>
   </si>
   <si>
-    <t>25676942</t>
+    <t>44926877</t>
+  </si>
+  <si>
+    <t>10270443</t>
+  </si>
+  <si>
+    <t>En trámite</t>
+  </si>
+  <si>
+    <t>placa</t>
+  </si>
+  <si>
+    <t>Consulta el numero de la poliza -Soat</t>
+  </si>
+  <si>
+    <t>@ConsultaNumeroDePolizaVehiSoat</t>
+  </si>
+  <si>
+    <t>@ConsultarDeudasSaldosdePoliza</t>
+  </si>
+  <si>
+    <t>Consultar Deudas y Saldos de la Poliza - Vehicular</t>
+  </si>
+  <si>
+    <t>AZG650</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -126,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,47 +174,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,15 +202,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -541,18 +531,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13795FAB-EE90-174B-9401-A5700886F2BE}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.6640625"/>
-    <col min="2" max="2" customWidth="true" width="37.6640625"/>
-    <col min="3" max="3" customWidth="true" width="77.1640625"/>
-    <col min="4" max="4" customWidth="true" style="3" width="8.1640625"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="77.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -570,13 +560,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -584,24 +574,50 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="14"/>
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="14"/>
+      <c r="B5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" location="DescargaPolizaVehicularDigital!A1" display="Aqui" xr:uid="{068FE6C9-3686-4C44-9A97-84A3A68C0290}"/>
     <hyperlink ref="D3" location="TiempoInactividadConsultaVehicu!A1" display="Aqui" xr:uid="{404AC63B-7694-0C4E-9C85-C0801828F6B1}"/>
+    <hyperlink ref="D4" location="ConsultaNumeroDePolizaVehiSoat!A1" display="Aqui" xr:uid="{FDE692C0-36D7-6444-BDC9-2C0103612732}"/>
+    <hyperlink ref="D5" location="ConsultarDeudasSaldosdePoliza!A1" display="Aqui" xr:uid="{2720FF6D-06C9-3146-9480-CD8A2E41DA6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -611,49 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4F0E03-958C-9E48-A583-3249367035D4}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81407C7-14F4-9E44-A012-97D01B607D5A}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,4 +664,145 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD64376-2D4E-6D41-B603-3C3AE1F6222D}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C2B533-22D6-0B45-821E-344598F85264}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81407C7-14F4-9E44-A012-97D01B607D5A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>